<commit_message>
relative path changes for odbc and excel path
</commit_message>
<xml_diff>
--- a/RestSharpFrameWork/Resources/Data.xlsx
+++ b/RestSharpFrameWork/Resources/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Spreadsheet SDK" lastEdited="1" lowestEdited="1" rupBuild="4.6.0.2025"/>
   <bookViews>
-    <workbookView autoFilterDateGrouping="1" xWindow="9192" yWindow="996" windowWidth="11952" windowHeight="8964" activeTab="2"/>
+    <workbookView autoFilterDateGrouping="1" xWindow="9195" yWindow="990" windowWidth="11955" windowHeight="8970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECTID" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>project_id</t>
   </si>
@@ -54,34 +54,34 @@
     <t>emp_Id</t>
   </si>
   <si>
-    <t>TYP_01452</t>
-  </si>
-  <si>
-    <t>TYP_01453</t>
-  </si>
-  <si>
-    <t>TYP_01454</t>
-  </si>
-  <si>
-    <t>TYP_01455</t>
-  </si>
-  <si>
-    <t>TYP_01456</t>
-  </si>
-  <si>
-    <t>TYP_01457</t>
-  </si>
-  <si>
-    <t>TYP_01458</t>
-  </si>
-  <si>
-    <t>TYP_01459</t>
-  </si>
-  <si>
-    <t>TYP_01460</t>
-  </si>
-  <si>
-    <t>TYP_01461</t>
+    <t>TYP_00202</t>
+  </si>
+  <si>
+    <t>TYP_00203</t>
+  </si>
+  <si>
+    <t>TYP_00204</t>
+  </si>
+  <si>
+    <t>TYP_00205</t>
+  </si>
+  <si>
+    <t>TYP_00206</t>
+  </si>
+  <si>
+    <t>TYP_00207</t>
+  </si>
+  <si>
+    <t>TYP_00208</t>
+  </si>
+  <si>
+    <t>TYP_00209</t>
+  </si>
+  <si>
+    <t>TYP_00210</t>
+  </si>
+  <si>
+    <t>TYP_00211</t>
   </si>
   <si>
     <t>createdBy</t>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Yasmin</t>
+  </si>
+  <si>
+    <t>yanittee</t>
   </si>
   <si>
     <t>Lakshmi</t>
@@ -318,7 +321,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -387,7 +390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -455,10 +458,10 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.29" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.71" style="1" customWidth="1"/>
@@ -526,7 +529,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>34</v>
@@ -537,10 +540,10 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>34</v>
@@ -551,10 +554,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>34</v>
@@ -565,10 +568,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>31</v>
@@ -579,10 +582,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>28</v>
@@ -593,10 +596,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>28</v>
@@ -607,10 +610,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>31</v>
@@ -633,7 +636,7 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.29" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.86" style="1" customWidth="1"/>
@@ -647,33 +650,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2">
         <v>4.1</v>
@@ -682,16 +685,16 @@
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H2" s="2">
         <v>9845632112</v>
@@ -699,7 +702,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2">
         <v>4.1</v>
@@ -708,16 +711,16 @@
         <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H3" s="2">
         <v>9845632113</v>
@@ -725,7 +728,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2">
         <v>4.1</v>
@@ -734,16 +737,16 @@
         <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H4" s="2">
         <v>9845632114</v>
@@ -751,7 +754,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2">
         <v>4.1</v>
@@ -760,16 +763,16 @@
         <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H5" s="2">
         <v>9845632115</v>
@@ -777,25 +780,25 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2">
         <v>4.1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H6" s="2">
         <v>9845632116</v>
@@ -803,25 +806,25 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2">
         <v>4.1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H7" s="2">
         <v>9845632117</v>
@@ -829,25 +832,25 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2">
         <v>4.1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H8" s="2">
         <v>9845632118</v>
@@ -855,25 +858,25 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2">
         <v>4.1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2">
         <v>9845632119</v>
@@ -881,25 +884,25 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2">
         <v>4.1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H10" s="2">
         <v>9845632120</v>
@@ -907,25 +910,25 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2">
         <v>4.1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H11" s="2">
         <v>9845632121</v>
@@ -955,81 +958,81 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" ht="15.6" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" ht="15.6" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="15.6" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" ht="15.6" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" ht="15.6" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" ht="15.6" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="15.6" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="15.6" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" ht="15.6" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" ht="15.6" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" ht="15.6" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>